<commit_message>
Update remaining templates's ontology terms
</commit_message>
<xml_diff>
--- a/templates/2EXT02_Protein/2EXT02_Protein.xlsx
+++ b/templates/2EXT02_Protein/2EXT02_Protein.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\2EXT02_Protein\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\2EXT02_Protein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F095B8-D584-4F7D-B843-35A4B0398A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF4F6E0-62D2-4587-845B-4256A599EDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT02_Protein" sheetId="1" r:id="rId1"/>
@@ -43,11 +43,11 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D96B17D5-C151-43C3-BAD3-4849955C8A0B}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The unique identifier of this template. It will be auto generated.
-Antwort:
+Reply:
     id=cf1fb06f-d72e-43d9-be25-4ea6c25f03e2</t>
       </text>
     </comment>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="144">
   <si>
     <t>Source Name</t>
   </si>
@@ -94,21 +94,9 @@
     <t>Parameter [staining]</t>
   </si>
   <si>
-    <t>Term Source REF (OBI:0302887)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (OBI:0302887)</t>
-  </si>
-  <si>
     <t>Parameter [buffer]</t>
   </si>
   <si>
-    <t>Term Source REF (CHEBI:35225)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (CHEBI:35225)</t>
-  </si>
-  <si>
     <t>Parameter [pH]</t>
   </si>
   <si>
@@ -133,12 +121,6 @@
     <t>Parameter [protein column]</t>
   </si>
   <si>
-    <t>Term Source REF (OBI:0000468)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (OBI:0000468)</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -433,7 +415,79 @@
     <t>Good's buffer substance</t>
   </si>
   <si>
-    <t>1.1.4</t>
+    <t>Term Source REF ()</t>
+  </si>
+  <si>
+    <t>Term Accession Number ()</t>
+  </si>
+  <si>
+    <t>Term Source REF ()2</t>
+  </si>
+  <si>
+    <t>Term Accession Number ()2</t>
+  </si>
+  <si>
+    <t>Term Source REF ()3</t>
+  </si>
+  <si>
+    <t>Term Accession Number ()3</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1001303</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1001251</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1001312</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1001955</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1001956</t>
+  </si>
+  <si>
+    <t>user-specific</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1003041</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000860</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1003015</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1003051</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000882</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1003036</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000047</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000051</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000052</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000048</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000050</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1000049</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
   </si>
 </sst>
 </file>
@@ -630,7 +684,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -670,11 +724,11 @@
     <tableColumn id="10" xr3:uid="{2AE81524-F7BC-4CED-BC6F-8FE76E960298}" name="Term Source REF (MS:1000003)"/>
     <tableColumn id="11" xr3:uid="{E89960B1-47E1-43FD-832D-D1E3FBF51F23}" name="Term Accession Number (MS:1000003)"/>
     <tableColumn id="12" xr3:uid="{9CA06C7C-058F-4B37-AC7A-12B3E4C63A5B}" name="Parameter [staining]"/>
-    <tableColumn id="13" xr3:uid="{BDF38729-6075-4DDC-92EC-18B22F924A5B}" name="Term Source REF (OBI:0302887)"/>
-    <tableColumn id="14" xr3:uid="{4C48CDEB-E2A1-4229-B3BA-5B9AF1B61DC0}" name="Term Accession Number (OBI:0302887)"/>
+    <tableColumn id="13" xr3:uid="{BDF38729-6075-4DDC-92EC-18B22F924A5B}" name="Term Source REF ()"/>
+    <tableColumn id="14" xr3:uid="{4C48CDEB-E2A1-4229-B3BA-5B9AF1B61DC0}" name="Term Accession Number ()"/>
     <tableColumn id="15" xr3:uid="{687A99E7-B6DD-4483-B15C-FB80607A1F17}" name="Parameter [buffer]"/>
-    <tableColumn id="16" xr3:uid="{278B5C07-179F-4E97-8082-8112D4A45914}" name="Term Source REF (CHEBI:35225)"/>
-    <tableColumn id="17" xr3:uid="{B51035F5-F3D6-48CC-BE83-F5A375E2289B}" name="Term Accession Number (CHEBI:35225)"/>
+    <tableColumn id="16" xr3:uid="{278B5C07-179F-4E97-8082-8112D4A45914}" name="Term Source REF ()2"/>
+    <tableColumn id="17" xr3:uid="{B51035F5-F3D6-48CC-BE83-F5A375E2289B}" name="Term Accession Number ()2"/>
     <tableColumn id="18" xr3:uid="{A76F4D4C-FBEC-4E1F-ABF1-313BBB6F55B7}" name="Parameter [pH]"/>
     <tableColumn id="21" xr3:uid="{78B7D35C-7FA9-4BC4-BECD-4CD211088C0D}" name="Unit" dataDxfId="0"/>
     <tableColumn id="19" xr3:uid="{8374D543-1198-4666-AE2A-72A23EA25666}" name="Term Source REF (UO:0000196)"/>
@@ -683,8 +737,8 @@
     <tableColumn id="31" xr3:uid="{0FDA3F08-732B-44E4-A593-E065B3A2582C}" name="Term Source REF (MS:1002493)"/>
     <tableColumn id="32" xr3:uid="{1755E1AD-351F-40BF-902C-735B0C443F5C}" name="Term Accession Number (MS:1002493)"/>
     <tableColumn id="33" xr3:uid="{480935E8-E049-46CA-8DA2-93D8D9C72DC6}" name="Parameter [protein column]"/>
-    <tableColumn id="34" xr3:uid="{1723442C-9032-4A69-B734-91DEEA704BFD}" name="Term Source REF (OBI:0000468)"/>
-    <tableColumn id="35" xr3:uid="{A1534108-7A55-4F03-A123-CA39CE80036C}" name="Term Accession Number (OBI:0000468)"/>
+    <tableColumn id="34" xr3:uid="{1723442C-9032-4A69-B734-91DEEA704BFD}" name="Term Source REF ()3"/>
+    <tableColumn id="35" xr3:uid="{A1534108-7A55-4F03-A123-CA39CE80036C}" name="Term Accession Number ()3"/>
     <tableColumn id="2" xr3:uid="{F18EF81D-B0BD-4C6E-A4BF-C5543EDB3CC7}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -965,7 +1019,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="667" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="678" row="2">
@@ -998,9 +1052,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
@@ -1066,49 +1120,49 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" t="s">
-        <v>24</v>
-      </c>
       <c r="Y1" t="s">
-        <v>25</v>
+        <v>123</v>
       </c>
       <c r="Z1" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="AA1" t="s">
         <v>1</v>
@@ -1116,82 +1170,208 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
         <v>104</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
         <v>110</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" t="s">
         <v>116</v>
       </c>
-      <c r="K2" t="s">
-        <v>122</v>
+      <c r="L2" t="s">
+        <v>130</v>
+      </c>
+      <c r="M2" t="s">
+        <v>130</v>
       </c>
       <c r="N2" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="O2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P2" t="s">
+        <v>130</v>
       </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
         <v>105</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" t="s">
         <v>111</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" t="s">
         <v>117</v>
       </c>
-      <c r="K3" t="s">
-        <v>123</v>
+      <c r="L3" t="s">
+        <v>130</v>
+      </c>
+      <c r="M3" t="s">
+        <v>130</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
         <v>106</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" t="s">
         <v>112</v>
       </c>
-      <c r="H4" t="s">
-        <v>118</v>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>139</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
         <v>107</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" t="s">
         <v>113</v>
       </c>
-      <c r="H5" t="s">
-        <v>119</v>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" t="s">
+        <v>140</v>
       </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" t="s">
         <v>108</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" t="s">
         <v>114</v>
       </c>
-      <c r="H6" t="s">
-        <v>120</v>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
+        <v>141</v>
       </c>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" t="s">
         <v>109</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" t="s">
         <v>115</v>
       </c>
-      <c r="H7" t="s">
-        <v>121</v>
+      <c r="I7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
       </c>
       <c r="R7" s="1"/>
     </row>
@@ -1208,9 +1388,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8F898E-70F9-4443-B417-1E256527228F}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.140625" customWidth="1"/>
@@ -1218,105 +1400,105 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="9"/>
@@ -1324,7 +1506,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="9"/>
@@ -1332,97 +1514,97 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="9"/>
@@ -1439,7 +1621,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -1457,40 +1639,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1498,13 +1680,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -1514,7 +1696,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1522,25 +1704,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1548,27 +1730,27 @@
         <v>5</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1576,27 +1758,27 @@
         <v>8</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1604,139 +1786,139 @@
         <v>11</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1744,13 +1926,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -1760,7 +1942,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>